<commit_message>
Renamed 'DATASET DESCRIPTION FILE' to 'SHORT DESCRIPTION FILE'
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -184,7 +184,7 @@
     <t xml:space="preserve">LICENSE URL</t>
   </si>
   <si>
-    <t xml:space="preserve">DATASET DESCRIPTION FILE</t>
+    <t xml:space="preserve">SHORT DESCRIPTION FILE</t>
   </si>
   <si>
     <t xml:space="preserve">NER</t>
@@ -742,7 +742,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -861,10 +861,10 @@
       <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.86"/>
@@ -5274,11 +5274,11 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10425,17 +10425,17 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -13753,9 +13753,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="134.14"/>
   </cols>
@@ -13914,11 +13914,11 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="118.73"/>
   </cols>
   <sheetData>
@@ -17117,7 +17117,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">

</xml_diff>

<commit_message>
Load dataset info from long descriptions file
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="160">
   <si>
     <t xml:space="preserve">HELP FOR ADDING A NEW SYSTEM/PAPER TO THE LEADERBOARD</t>
   </si>
@@ -187,6 +187,9 @@
     <t xml:space="preserve">SHORT DESCRIPTION FILE</t>
   </si>
   <si>
+    <t xml:space="preserve">LONG DESCRIPTION FILE</t>
+  </si>
+  <si>
     <t xml:space="preserve">NER</t>
   </si>
   <si>
@@ -202,6 +205,9 @@
     <t xml:space="preserve">MIT</t>
   </si>
   <si>
+    <t xml:space="preserve">RONEC-v1.0-site.md</t>
+  </si>
+  <si>
     <t xml:space="preserve">RONEC-v1.0.md</t>
   </si>
   <si>
@@ -215,6 +221,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://creativecommons.org/licenses/by-sa/4.0/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniversalDependencies-RO-RRT-v2.5-site.md</t>
   </si>
   <si>
     <t xml:space="preserve">UniversalDependencies-RO-RRT-v2.5.md</t>
@@ -250,6 +259,9 @@
     <t xml:space="preserve">LaRoSeDa-site.md</t>
   </si>
   <si>
+    <t xml:space="preserve">LaRoSeDa.md</t>
+  </si>
+  <si>
     <t xml:space="preserve">Text Classification</t>
   </si>
   <si>
@@ -257,6 +269,9 @@
   </si>
   <si>
     <t xml:space="preserve">MOROCO-site.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOROCO.md</t>
   </si>
   <si>
     <t xml:space="preserve">AREA</t>
@@ -10426,7 +10441,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10437,6 +10452,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -10462,7 +10478,9 @@
       <c r="G1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="10"/>
+      <c r="H1" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -10474,174 +10492,198 @@
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="G9" s="11" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13762,134 +13804,134 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -13924,94 +13966,94 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14019,13 +14061,13 @@
         <v>44</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14033,13 +14075,13 @@
         <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14047,13 +14089,13 @@
         <v>40</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14061,13 +14103,13 @@
         <v>41</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14075,27 +14117,27 @@
         <v>42</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14103,41 +14145,41 @@
         <v>43</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17121,253 +17163,253 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed NLP area to NLP Benchmark
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Help-ReadMeFirst" sheetId="1" state="visible" r:id="rId2"/>
@@ -319,7 +319,7 @@
     <t xml:space="preserve">DESCRIPTION</t>
   </si>
   <si>
-    <t xml:space="preserve">NLP</t>
+    <t xml:space="preserve">NLP Benchmark</t>
   </si>
   <si>
     <t xml:space="preserve">Text Categorization by Topic</t>
@@ -904,7 +904,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1023,7 +1023,7 @@
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
@@ -5721,11 +5721,11 @@
   </sheetPr>
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11037,11 +11037,11 @@
   </sheetPr>
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11357,9 +11357,9 @@
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.29"/>
@@ -14898,7 +14898,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -18154,10 +18154,10 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
   </cols>

</xml_diff>

<commit_message>
Added column Remarks to Areas sheet
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Help-ReadMeFirst" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="193">
   <si>
     <t xml:space="preserve">HELP FOR ADDING A NEW SYSTEM/PAPER TO THE LEADERBOARD</t>
   </si>
@@ -599,6 +599,12 @@
   </si>
   <si>
     <t xml:space="preserve">RANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMARKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not part of the official benchmark.</t>
   </si>
 </sst>
 </file>
@@ -904,7 +910,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1023,7 +1029,7 @@
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
@@ -5725,7 +5731,7 @@
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11037,11 +11043,11 @@
   </sheetPr>
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11357,7 +11363,7 @@
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
@@ -14898,7 +14904,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -18153,13 +18159,14 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18169,6 +18176,9 @@
       <c r="B1" s="5" t="s">
         <v>190</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -18184,6 +18194,9 @@
       </c>
       <c r="B3" s="3" t="n">
         <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated source for Romanian Word Embeddings dataset
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Help-ReadMeFirst" sheetId="1" state="visible" r:id="rId2"/>
@@ -517,7 +517,7 @@
     <t xml:space="preserve">https://dumps.wikimedia.org/rowiki/20210401/</t>
   </si>
   <si>
-    <t xml:space="preserve">https://corola.racai.ro/</t>
+    <t xml:space="preserve">https://github.com/LiroBenchmark/gender-bias/tree/main/embeddings_ro</t>
   </si>
   <si>
     <t xml:space="preserve">METRICS</t>
@@ -910,7 +910,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1029,14 +1029,13 @@
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.71"/>
   </cols>
   <sheetData>
@@ -5727,11 +5726,11 @@
   </sheetPr>
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11047,7 +11046,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11360,14 +11359,14 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.7"/>
@@ -14881,7 +14880,7 @@
     <hyperlink ref="C15" r:id="rId25" display="https://universaldependencies.org/"/>
     <hyperlink ref="F15" r:id="rId26" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
     <hyperlink ref="C16" r:id="rId27" display="https://dumps.wikimedia.org/rowiki/20210401/"/>
-    <hyperlink ref="C17" r:id="rId28" display="https://corola.racai.ro/"/>
+    <hyperlink ref="C17" r:id="rId28" display="https://github.com/LiroBenchmark/gender-bias/tree/main/embeddings_ro"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -14904,7 +14903,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -18159,11 +18158,11 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.8"/>

</xml_diff>

<commit_message>
Updated leaderboard to fetch info from new dataset description files
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Help-ReadMeFirst" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="197">
   <si>
     <t xml:space="preserve">HELP FOR ADDING A NEW SYSTEM/PAPER TO THE LEADERBOARD</t>
   </si>
@@ -517,7 +517,19 @@
     <t xml:space="preserve">https://dumps.wikimedia.org/rowiki/20210401/</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/LiroBenchmark/gender-bias/tree/main/embeddings_ro</t>
+    <t xml:space="preserve">Wiki-ro-site.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiki-ro.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/LiroBenchmark/gender-bias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">romanian-word-embeddings.site.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">romanian-word-embeddings.md</t>
   </si>
   <si>
     <t xml:space="preserve">METRICS</t>
@@ -910,7 +922,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1029,7 +1041,7 @@
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
@@ -5726,11 +5738,11 @@
   </sheetPr>
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11046,7 +11058,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11358,11 +11370,11 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
@@ -11788,6 +11800,12 @@
       <c r="F16" s="7" t="s">
         <v>157</v>
       </c>
+      <c r="G16" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
@@ -11797,7 +11815,7 @@
         <v>75</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>93</v>
@@ -11807,6 +11825,12 @@
       </c>
       <c r="F17" s="0" t="s">
         <v>157</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14880,7 +14904,7 @@
     <hyperlink ref="C15" r:id="rId25" display="https://universaldependencies.org/"/>
     <hyperlink ref="F15" r:id="rId26" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
     <hyperlink ref="C16" r:id="rId27" display="https://dumps.wikimedia.org/rowiki/20210401/"/>
-    <hyperlink ref="C17" r:id="rId28" display="https://github.com/LiroBenchmark/gender-bias/tree/main/embeddings_ro"/>
+    <hyperlink ref="C17" r:id="rId28" display="https://github.com/LiroBenchmark/gender-bias"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -14903,7 +14927,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -14913,13 +14937,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>96</v>
@@ -14930,47 +14954,47 @@
         <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14978,13 +15002,13 @@
         <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14992,13 +15016,13 @@
         <v>89</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15006,13 +15030,13 @@
         <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15020,13 +15044,13 @@
         <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15034,13 +15058,13 @@
         <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15048,13 +15072,13 @@
         <v>80</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15062,13 +15086,13 @@
         <v>81</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15076,27 +15100,27 @@
         <v>82</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15104,27 +15128,27 @@
         <v>83</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15132,13 +15156,13 @@
         <v>90</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15146,27 +15170,27 @@
         <v>91</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15174,13 +15198,13 @@
         <v>87</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15188,13 +15212,13 @@
         <v>93</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18162,7 +18186,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.8"/>
@@ -18173,10 +18197,10 @@
         <v>95</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18195,7 +18219,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Link Cross-Domain tasks with their descriptions
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="199">
   <si>
     <t xml:space="preserve">HELP FOR ADDING A NEW SYSTEM/PAPER TO THE LEADERBOARD</t>
   </si>
@@ -512,6 +512,12 @@
   </si>
   <si>
     <t xml:space="preserve">XQuAD-ro.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniversalDependencies-RO-RRT-v2.8-Cross-Domain-site.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniversalDependencies-RO-RRT-v2.8-Cross-Domain.md</t>
   </si>
   <si>
     <t xml:space="preserve">https://dumps.wikimedia.org/rowiki/20210401/</t>
@@ -922,7 +928,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1041,7 +1047,7 @@
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
@@ -5742,7 +5748,7 @@
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11058,7 +11064,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11371,10 +11377,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
@@ -11749,10 +11755,10 @@
         <v>141</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11775,10 +11781,10 @@
         <v>141</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11789,7 +11795,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>92</v>
@@ -11801,10 +11807,10 @@
         <v>157</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11815,7 +11821,7 @@
         <v>75</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>93</v>
@@ -11827,10 +11833,10 @@
         <v>157</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14904,7 +14910,7 @@
     <hyperlink ref="C15" r:id="rId25" display="https://universaldependencies.org/"/>
     <hyperlink ref="F15" r:id="rId26" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
     <hyperlink ref="C16" r:id="rId27" display="https://dumps.wikimedia.org/rowiki/20210401/"/>
-    <hyperlink ref="C17" r:id="rId28" display="https://github.com/LiroBenchmark/gender-bias"/>
+    <hyperlink ref="C17" r:id="rId28" display="https://github.com/LiroBenchmark/gender-bias "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -14927,7 +14933,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -14937,13 +14943,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>96</v>
@@ -14954,47 +14960,47 @@
         <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15002,13 +15008,13 @@
         <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15016,13 +15022,13 @@
         <v>89</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15030,13 +15036,13 @@
         <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15044,13 +15050,13 @@
         <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15058,13 +15064,13 @@
         <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15072,13 +15078,13 @@
         <v>80</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15086,13 +15092,13 @@
         <v>81</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15100,27 +15106,27 @@
         <v>82</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15128,27 +15134,27 @@
         <v>83</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15156,13 +15162,13 @@
         <v>90</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15170,27 +15176,27 @@
         <v>91</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15198,13 +15204,13 @@
         <v>87</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15212,13 +15218,13 @@
         <v>93</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18186,7 +18192,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.8"/>
@@ -18197,10 +18203,10 @@
         <v>95</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18219,7 +18225,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated name for cross-domain tasks
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help-ReadMeFirst" sheetId="1" state="visible" r:id="rId2"/>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">https://github.com/ancatache/LaRoSeDa</t>
   </si>
   <si>
-    <t xml:space="preserve">UD Romanian RRT Treebank v2.5 – cross-domain PoS tagging</t>
+    <t xml:space="preserve">UD Romanian RRT Treebank v2.8 – cross-domain PoS tagging</t>
   </si>
   <si>
     <t xml:space="preserve">LiRo Baseline Stanza</t>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">https://openreview.net/forum?id=JH61CD7afTv</t>
   </si>
   <si>
-    <t xml:space="preserve">UD Romanian RRT Treebank v2.5 – cross-domain Dependency Parsing</t>
+    <t xml:space="preserve">UD Romanian RRT Treebank v2.8 – cross-domain Dependency Parsing</t>
   </si>
   <si>
     <t xml:space="preserve">RONEC - Romanian Named Entity Corpus v1.0</t>
@@ -928,7 +928,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1043,11 +1043,11 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
@@ -5745,10 +5745,10 @@
   <dimension ref="A1:D997"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11064,7 +11064,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11376,11 +11376,11 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
@@ -14933,7 +14933,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -18192,7 +18192,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.8"/>

</xml_diff>

<commit_message>
Updated source link for Wiki-Ro dataset
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Help-ReadMeFirst" sheetId="1" state="visible" r:id="rId2"/>
@@ -520,7 +520,7 @@
     <t xml:space="preserve">UniversalDependencies-RO-RRT-v2.8-Cross-Domain.md</t>
   </si>
   <si>
-    <t xml:space="preserve">https://dumps.wikimedia.org/rowiki/20210401/</t>
+    <t xml:space="preserve">https://github.com/dumitrescustefan/wiki-ro</t>
   </si>
   <si>
     <t xml:space="preserve">Wiki-ro-site.md</t>
@@ -928,7 +928,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1043,11 +1043,11 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
@@ -5748,7 +5748,7 @@
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11064,7 +11064,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11376,11 +11376,11 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
@@ -14909,7 +14909,7 @@
     <hyperlink ref="F14" r:id="rId24" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
     <hyperlink ref="C15" r:id="rId25" display="https://universaldependencies.org/"/>
     <hyperlink ref="F15" r:id="rId26" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C16" r:id="rId27" display="https://dumps.wikimedia.org/rowiki/20210401/"/>
+    <hyperlink ref="C16" r:id="rId27" display="https://github.com/dumitrescustefan/wiki-ro"/>
     <hyperlink ref="C17" r:id="rId28" display="https://github.com/LiroBenchmark/gender-bias "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14933,7 +14933,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -18192,7 +18192,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.8"/>

</xml_diff>

<commit_message>
Updated licence for Wiki-Ro dataset
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="200">
   <si>
     <t xml:space="preserve">HELP FOR ADDING A NEW SYSTEM/PAPER TO THE LEADERBOARD</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t xml:space="preserve">MIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mit-license.org/</t>
   </si>
   <si>
     <t xml:space="preserve">RONEC-v1.0-site.md</t>
@@ -928,7 +931,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1047,7 +1050,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
@@ -5748,7 +5751,7 @@
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11064,7 +11067,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11377,10 +11380,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
@@ -11426,7 +11429,7 @@
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>100</v>
       </c>
@@ -11442,11 +11445,14 @@
       <c r="E2" s="3" t="s">
         <v>136</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>137</v>
+      </c>
       <c r="G2" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11457,22 +11463,22 @@
         <v>27</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11483,22 +11489,22 @@
         <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11509,22 +11515,22 @@
         <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11535,22 +11541,22 @@
         <v>23</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11561,22 +11567,22 @@
         <v>35</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11593,16 +11599,16 @@
         <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11613,22 +11619,22 @@
         <v>52</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11645,16 +11651,16 @@
         <v>88</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11662,7 +11668,7 @@
         <v>102</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>49</v>
@@ -11671,16 +11677,16 @@
         <v>91</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11691,22 +11697,22 @@
         <v>42</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11723,16 +11729,16 @@
         <v>86</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11743,22 +11749,22 @@
         <v>61</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11769,22 +11775,22 @@
         <v>65</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>84</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11795,22 +11801,22 @@
         <v>73</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>92</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11821,22 +11827,22 @@
         <v>75</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>93</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14884,33 +14890,35 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://github.com/dumitrescustefan/ronec"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://universaldependencies.org/"/>
-    <hyperlink ref="F3" r:id="rId3" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C4" r:id="rId4" display="https://universaldependencies.org/"/>
-    <hyperlink ref="F4" r:id="rId5" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C5" r:id="rId6" display="https://universaldependencies.org/"/>
-    <hyperlink ref="F5" r:id="rId7" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C6" r:id="rId8" display="https://universaldependencies.org/"/>
-    <hyperlink ref="F6" r:id="rId9" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C7" r:id="rId10" display="https://universaldependencies.org/"/>
-    <hyperlink ref="F7" r:id="rId11" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C8" r:id="rId12" display="https://github.com/ancatache/LaRoSeDa"/>
-    <hyperlink ref="F8" r:id="rId13" display="https://creativecommons.org/licenses/by-nc-sa/4.0/"/>
-    <hyperlink ref="C9" r:id="rId14" display="https://github.com/butnaruandrei/MOROCO"/>
-    <hyperlink ref="F9" r:id="rId15" display="https://creativecommons.org/licenses/by-nc-sa/4.0/"/>
-    <hyperlink ref="C10" r:id="rId16" display="https://github.com/dumitrescustefan/RO-STS"/>
-    <hyperlink ref="F10" r:id="rId17" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C11" r:id="rId18" display="https://github.com/dumitrescustefan/RO-STS"/>
-    <hyperlink ref="F11" r:id="rId19" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C12" r:id="rId20" location="download" display="https://www.statmt.org/wmt16/translation-task.html#download"/>
-    <hyperlink ref="C13" r:id="rId21" display="https://github.com/deepmind/xquad"/>
-    <hyperlink ref="F13" r:id="rId22" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C14" r:id="rId23" display="https://universaldependencies.org/"/>
-    <hyperlink ref="F14" r:id="rId24" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C15" r:id="rId25" display="https://universaldependencies.org/"/>
-    <hyperlink ref="F15" r:id="rId26" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
-    <hyperlink ref="C16" r:id="rId27" display="https://github.com/dumitrescustefan/wiki-ro"/>
-    <hyperlink ref="C17" r:id="rId28" display="https://github.com/LiroBenchmark/gender-bias "/>
+    <hyperlink ref="F2" r:id="rId2" display="https://mit-license.org/"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://universaldependencies.org/"/>
+    <hyperlink ref="F3" r:id="rId4" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C4" r:id="rId5" display="https://universaldependencies.org/"/>
+    <hyperlink ref="F4" r:id="rId6" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C5" r:id="rId7" display="https://universaldependencies.org/"/>
+    <hyperlink ref="F5" r:id="rId8" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C6" r:id="rId9" display="https://universaldependencies.org/"/>
+    <hyperlink ref="F6" r:id="rId10" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C7" r:id="rId11" display="https://universaldependencies.org/"/>
+    <hyperlink ref="F7" r:id="rId12" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C8" r:id="rId13" display="https://github.com/ancatache/LaRoSeDa"/>
+    <hyperlink ref="F8" r:id="rId14" display="https://creativecommons.org/licenses/by-nc-sa/4.0/"/>
+    <hyperlink ref="C9" r:id="rId15" display="https://github.com/butnaruandrei/MOROCO"/>
+    <hyperlink ref="F9" r:id="rId16" display="https://creativecommons.org/licenses/by-nc-sa/4.0/"/>
+    <hyperlink ref="C10" r:id="rId17" display="https://github.com/dumitrescustefan/RO-STS"/>
+    <hyperlink ref="F10" r:id="rId18" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C11" r:id="rId19" display="https://github.com/dumitrescustefan/RO-STS"/>
+    <hyperlink ref="F11" r:id="rId20" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C12" r:id="rId21" location="download" display="https://www.statmt.org/wmt16/translation-task.html#download"/>
+    <hyperlink ref="C13" r:id="rId22" display="https://github.com/deepmind/xquad"/>
+    <hyperlink ref="F13" r:id="rId23" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C14" r:id="rId24" display="https://universaldependencies.org/"/>
+    <hyperlink ref="F14" r:id="rId25" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C15" r:id="rId26" display="https://universaldependencies.org/"/>
+    <hyperlink ref="F15" r:id="rId27" display="https://creativecommons.org/licenses/by-sa/4.0/"/>
+    <hyperlink ref="C16" r:id="rId28" display="https://github.com/dumitrescustefan/wiki-ro"/>
+    <hyperlink ref="F16" r:id="rId29" display="https://mit-license.org/"/>
+    <hyperlink ref="C17" r:id="rId30" display="https://github.com/LiroBenchmark/gender-bias "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -14933,7 +14941,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -14943,13 +14951,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>96</v>
@@ -14960,47 +14968,47 @@
         <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15008,13 +15016,13 @@
         <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15022,13 +15030,13 @@
         <v>89</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15036,13 +15044,13 @@
         <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15050,13 +15058,13 @@
         <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15064,13 +15072,13 @@
         <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15078,13 +15086,13 @@
         <v>80</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15092,13 +15100,13 @@
         <v>81</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15106,27 +15114,27 @@
         <v>82</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15134,27 +15142,27 @@
         <v>83</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15162,13 +15170,13 @@
         <v>90</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15176,27 +15184,27 @@
         <v>91</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>193</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15204,13 +15212,13 @@
         <v>87</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15218,13 +15226,13 @@
         <v>93</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18192,7 +18200,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.8"/>
@@ -18203,10 +18211,10 @@
         <v>95</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18225,7 +18233,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated licence for Romanian Word Embeddings
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="202">
   <si>
     <t xml:space="preserve">HELP FOR ADDING A NEW SYSTEM/PAPER TO THE LEADERBOARD</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/LiroBenchmark/gender-bias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC BY-NC 4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://creativecommons.org/licenses/by-nc/4.0/</t>
   </si>
   <si>
     <t xml:space="preserve">romanian-word-embeddings.site.md</t>
@@ -931,7 +937,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1050,7 +1056,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
@@ -5751,7 +5757,7 @@
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.98"/>
@@ -11067,7 +11073,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.28"/>
@@ -11380,10 +11386,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.29"/>
@@ -11833,16 +11839,16 @@
         <v>93</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14919,6 +14925,7 @@
     <hyperlink ref="C16" r:id="rId28" display="https://github.com/dumitrescustefan/wiki-ro"/>
     <hyperlink ref="F16" r:id="rId29" display="https://mit-license.org/"/>
     <hyperlink ref="C17" r:id="rId30" display="https://github.com/LiroBenchmark/gender-bias "/>
+    <hyperlink ref="F17" r:id="rId31" display="https://creativecommons.org/licenses/by-nc/4.0/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -14941,7 +14948,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.42"/>
@@ -14951,13 +14958,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>96</v>
@@ -14968,47 +14975,47 @@
         <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15016,13 +15023,13 @@
         <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15030,13 +15037,13 @@
         <v>89</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15044,13 +15051,13 @@
         <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15058,13 +15065,13 @@
         <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15072,13 +15079,13 @@
         <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15086,13 +15093,13 @@
         <v>80</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15100,13 +15107,13 @@
         <v>81</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15114,27 +15121,27 @@
         <v>82</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15142,27 +15149,27 @@
         <v>83</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15170,13 +15177,13 @@
         <v>90</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15184,27 +15191,27 @@
         <v>91</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15212,13 +15219,13 @@
         <v>87</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15226,13 +15233,13 @@
         <v>93</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18200,7 +18207,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.8"/>
@@ -18211,10 +18218,10 @@
         <v>95</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18233,7 +18240,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added REDv2 + results
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\personal\liro\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\personal\liro-fork\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA922F78-3961-4A4D-9642-F432FC491EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF29F09A-AB33-4B73-B6DE-50CED935474E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Help-ReadMeFirst" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="213">
   <si>
     <t>HELP FOR ADDING A NEW SYSTEM/PAPER TO THE LEADERBOARD</t>
   </si>
@@ -192,9 +192,6 @@
     <t>https://github.com/dumitrescustefan/RO-STS</t>
   </si>
   <si>
-    <t>RO-STS Baseline Romanian BERT v1 (uncased)</t>
-  </si>
-  <si>
     <t>RO-STS Baseline mBERT (uncased)</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>RONEC - Romanian Named Entity Corpus v1.0</t>
   </si>
   <si>
-    <t>Romanian BERT Baseline</t>
-  </si>
-  <si>
     <t>The birth of Romanian BERT</t>
   </si>
   <si>
@@ -264,9 +258,6 @@
     <t>Wiki-Ro</t>
   </si>
   <si>
-    <t>LiRo Baseline ro-Bert</t>
-  </si>
-  <si>
     <t>Romanian word embeddings</t>
   </si>
   <si>
@@ -315,9 +306,6 @@
     <t>Spearman Correlation</t>
   </si>
   <si>
-    <t>Exact Match F1</t>
-  </si>
-  <si>
     <t>BLEU</t>
   </si>
   <si>
@@ -658,13 +646,46 @@
   </si>
   <si>
     <t>Natural Language Processing</t>
+  </si>
+  <si>
+    <t>bert-base-romanian-cased-v1</t>
+  </si>
+  <si>
+    <t>bert-base-romanian-uncased-v1</t>
+  </si>
+  <si>
+    <t>Romanian Emotions Datasets v2 (REDv2)</t>
+  </si>
+  <si>
+    <t>https://github.com/Alegzandra/RED-Romanian-Emotions-Dataset</t>
+  </si>
+  <si>
+    <t>Hamming Loss</t>
+  </si>
+  <si>
+    <t>[0, 1]</t>
+  </si>
+  <si>
+    <t>For multi-label classification problems like REDv2</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>[0, INFINITY]</t>
+  </si>
+  <si>
+    <t>General purpose Mean Squared Error</t>
+  </si>
+  <si>
+    <t>dumitrescustefan/Romanian-Transformers: This repo is the home of Romanian Transformers. (github.com)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -726,6 +747,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -760,7 +793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -786,6 +819,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1281,7 +1318,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1333,8 +1370,8 @@
       <c r="E2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>26</v>
+      <c r="F2" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="G2" s="3">
         <v>5</v>
@@ -1712,7 +1749,7 @@
         <v>47</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>50</v>
+        <v>203</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>49</v>
@@ -1735,7 +1772,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>49</v>
@@ -1755,16 +1792,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="C19" t="s">
         <v>53</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>32</v>
@@ -1778,19 +1815,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="C20" t="s">
         <v>57</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>32</v>
@@ -1804,16 +1841,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="C21" t="s">
         <v>62</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>63</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>32</v>
@@ -1827,16 +1864,16 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
         <v>62</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>63</v>
-      </c>
-      <c r="D22" t="s">
-        <v>64</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>32</v>
@@ -1850,16 +1887,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="D23" t="s">
         <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
       </c>
       <c r="E23" t="s">
         <v>25</v>
@@ -1879,13 +1916,13 @@
         <v>42</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
         <v>70</v>
-      </c>
-      <c r="C24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" t="s">
-        <v>72</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>32</v>
@@ -1899,16 +1936,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>74</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
         <v>63</v>
-      </c>
-      <c r="D25" t="s">
-        <v>64</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>32</v>
@@ -1922,19 +1959,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
         <v>63</v>
       </c>
-      <c r="D26" t="s">
-        <v>64</v>
-      </c>
       <c r="E26" s="19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>32</v>
@@ -1947,9 +1984,18 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-      <c r="B27" s="12"/>
-      <c r="F27" s="8"/>
+      <c r="A27" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
@@ -5963,6 +6009,7 @@
     <hyperlink ref="D25" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
     <hyperlink ref="D26" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
     <hyperlink ref="E26" r:id="rId39" xr:uid="{2A7D20E5-2197-4AD7-8193-1F1BDE96EC46}"/>
+    <hyperlink ref="E27" r:id="rId40" display="https://github.com/dumitrescustefan/Romanian-Transformers" xr:uid="{17A5440C-2431-4AC5-985A-95784E369F4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5989,7 +6036,7 @@
   <dimension ref="A1:D997"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -6001,16 +6048,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -6021,7 +6068,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3">
         <v>99.74</v>
@@ -6035,7 +6082,7 @@
         <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3">
         <v>95.56</v>
@@ -6049,7 +6096,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3">
         <v>96.91</v>
@@ -6063,7 +6110,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3">
         <v>97.42</v>
@@ -6077,7 +6124,7 @@
         <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" s="3">
         <v>90.38</v>
@@ -6091,7 +6138,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D7" s="3">
         <v>85.23</v>
@@ -6105,7 +6152,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D8" s="3">
         <v>99.71</v>
@@ -6119,7 +6166,7 @@
         <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3">
         <v>95.42</v>
@@ -6133,7 +6180,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" s="3">
         <v>96.57</v>
@@ -6147,7 +6194,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D11" s="3">
         <v>96.96</v>
@@ -6161,7 +6208,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D12" s="3">
         <v>90.14</v>
@@ -6175,7 +6222,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D13" s="3">
         <v>85.06</v>
@@ -6189,7 +6236,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D14" s="3">
         <v>98.18</v>
@@ -6203,7 +6250,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D15" s="3">
         <v>72.7</v>
@@ -6217,7 +6264,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D16" s="3">
         <v>83.6</v>
@@ -6231,7 +6278,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D17" s="3">
         <v>59.9</v>
@@ -6245,7 +6292,7 @@
         <v>37</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D18" s="3">
         <v>69.7</v>
@@ -6259,7 +6306,7 @@
         <v>47</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D19">
         <v>0.6744</v>
@@ -6273,7 +6320,7 @@
         <v>47</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D20">
         <v>0.66620000000000001</v>
@@ -6281,13 +6328,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>50</v>
+        <v>203</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D21">
         <v>0.81589999999999996</v>
@@ -6295,13 +6342,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>50</v>
+        <v>203</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D22">
         <v>0.80859999999999999</v>
@@ -6309,13 +6356,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D23">
         <v>0.76900000000000002</v>
@@ -6323,13 +6370,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D24">
         <v>0.76500000000000001</v>
@@ -6337,13 +6384,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D25">
         <v>88.03</v>
@@ -6351,13 +6398,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D26">
         <v>54.3</v>
@@ -6365,13 +6412,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D27">
         <v>95.73</v>
@@ -6379,13 +6426,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <v>88.97</v>
@@ -6393,27 +6440,27 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>67</v>
+        <v>202</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>91</v>
+        <v>198</v>
       </c>
       <c r="D29">
-        <v>85.88</v>
+        <v>88.15</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D30">
         <v>38.5</v>
@@ -6421,13 +6468,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
-        <v>74</v>
+        <v>202</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D31">
         <v>28</v>
@@ -6435,94 +6482,103 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D32">
         <v>2.57</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D33">
+        <v>0.1038</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -11316,7 +11372,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -11328,245 +11384,247 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="5" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="11" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="12" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="13" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="14" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C14" s="15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B11" s="3" t="s">
+    <row r="15" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C15" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B13" s="10" t="s">
+    <row r="16" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="B16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="8"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="8"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="8"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
+    <row r="17" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+    </row>
+    <row r="18" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="22"/>
+    </row>
+    <row r="19" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="22"/>
+    </row>
+    <row r="20" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="22"/>
+    </row>
+    <row r="21" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="22"/>
+    </row>
+    <row r="22" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="22"/>
+    </row>
+    <row r="23" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="22"/>
+    </row>
+    <row r="24" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="22"/>
+    </row>
+    <row r="25" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="22"/>
+    </row>
+    <row r="26" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="22"/>
+    </row>
+    <row r="28" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="22"/>
+    </row>
+    <row r="29" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="22"/>
+    </row>
+    <row r="30" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="22"/>
+    </row>
+    <row r="31" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="22"/>
+    </row>
+    <row r="32" spans="1:3" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="22"/>
+    </row>
+    <row r="33" spans="1:1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="22"/>
+    </row>
+    <row r="34" spans="1:1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="22"/>
+    </row>
+    <row r="35" spans="1:1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="22"/>
+    </row>
+    <row r="36" spans="1:1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37" spans="1:1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38" spans="1:1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="22"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
@@ -11608,6 +11666,9 @@
       <c r="A51" s="8"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C16">
+    <sortCondition ref="A2:A16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
@@ -11632,8 +11693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -11650,31 +11711,31 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="H1" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>135</v>
       </c>
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
@@ -11687,223 +11748,223 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="18" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="18" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>47</v>
@@ -11912,79 +11973,79 @@
         <v>49</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>37</v>
@@ -11993,135 +12054,151 @@
         <v>40</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="18" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="18" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C17" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I17" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" t="s">
-        <v>168</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" t="s">
-        <v>170</v>
-      </c>
-      <c r="I17" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="A18" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
@@ -15185,6 +15262,8 @@
     <hyperlink ref="C17" r:id="rId30" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
     <hyperlink ref="F17" r:id="rId31" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
     <hyperlink ref="G17" r:id="rId32" xr:uid="{0960FD31-EB67-4DB5-9CE0-15EA9670F4D0}"/>
+    <hyperlink ref="C18" r:id="rId33" xr:uid="{D40EA6B2-3165-482B-8419-A53941311FDC}"/>
+    <hyperlink ref="F18" r:id="rId34" xr:uid="{4072F152-F7D5-4682-B895-3AD201680196}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -15220,7 +15299,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -15233,295 +15312,317 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="8"/>
+      <c r="A22" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="8"/>
+      <c r="A23" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B24" s="8"/>
@@ -18470,8 +18571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -18482,18 +18583,18 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -18501,13 +18602,13 @@
     </row>
     <row r="3" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update REDv2 citation and site description
</commit_message>
<xml_diff>
--- a/src/data/LEADERBOARD.xlsx
+++ b/src/data/LEADERBOARD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\personal\liro-fork\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D39EF9-150E-460C-87CC-95ABC11012A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5320ED5-5803-4903-B5D4-40EBD77BBD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="214">
   <si>
     <t>HELP FOR ADDING A NEW SYSTEM/PAPER TO THE LEADERBOARD</t>
   </si>
@@ -675,7 +675,13 @@
     <t>General purpose Mean Squared Error</t>
   </si>
   <si>
-    <t>dumitrescustefan/Romanian-Transformers: This repo is the home of Romanian Transformers. (github.com)</t>
+    <t>http://www.lrec-conf.org/proceedings/lrec2022/pdf/2022.lrec-1.149.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/Alegzandra/RED-Romanian-Emotions-Dataset/tree/main/REDv2</t>
+  </si>
+  <si>
+    <t>RED v2: Enhancing RED Dataset for Multi-Label Emotion Detection</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1321,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1689,7 +1695,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>42</v>
       </c>
@@ -1993,8 +1999,14 @@
       <c r="B27" s="14" t="s">
         <v>202</v>
       </c>
+      <c r="C27" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>211</v>
+      </c>
       <c r="E27" s="19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F27" s="23" t="s">
         <v>32</v>
@@ -6021,7 +6033,8 @@
     <hyperlink ref="D25" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
     <hyperlink ref="D26" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
     <hyperlink ref="E26" r:id="rId39" xr:uid="{2A7D20E5-2197-4AD7-8193-1F1BDE96EC46}"/>
-    <hyperlink ref="E27" r:id="rId40" display="https://github.com/dumitrescustefan/Romanian-Transformers" xr:uid="{17A5440C-2431-4AC5-985A-95784E369F4B}"/>
+    <hyperlink ref="E27" r:id="rId40" xr:uid="{17A5440C-2431-4AC5-985A-95784E369F4B}"/>
+    <hyperlink ref="D27" r:id="rId41" xr:uid="{187F2126-33BE-4674-ADA8-668E6EACA0A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>